<commit_message>
implementation; ergebnisse; kleine korrekturen
</commit_message>
<xml_diff>
--- a/raw/DNSBenchResults.xlsx
+++ b/raw/DNSBenchResults.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28605" windowHeight="13710" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28605" windowHeight="13710" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Uncached" sheetId="2" r:id="rId2"/>
-    <sheet name="Chart1" sheetId="3" r:id="rId3"/>
+    <sheet name="Knot_Uncached_Data" sheetId="4" r:id="rId2"/>
+    <sheet name="Knot_Uncached_Chart" sheetId="5" r:id="rId3"/>
+    <sheet name="Unbound_Uncached_Data" sheetId="2" r:id="rId4"/>
+    <sheet name="Unbound_Uncached_Chart" sheetId="3" r:id="rId5"/>
+    <sheet name="Mixed_Chart" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
-  <si>
-    <t>Resolver IP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="28">
   <si>
     <t>Resolver Type</t>
   </si>
@@ -87,13 +88,40 @@
   <si>
     <t>Forward Lookup with UDP</t>
   </si>
+  <si>
+    <t>Resolver Software</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Unbound 1.7.3 (Openssl 1.1.0h-fips)</t>
+  </si>
+  <si>
+    <t>Knot-Resolver 2.4.1</t>
+  </si>
+  <si>
+    <t>Unknown (Quad9)</t>
+  </si>
+  <si>
+    <t>Unbound</t>
+  </si>
+  <si>
+    <t>Knot Resolver</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -132,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -164,25 +192,235 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -221,7 +459,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Uncached!$B$1</c:f>
+              <c:f>Knot_Uncached_Data!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -242,14 +480,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Uncached!$A$2:$A$4</c:f>
+              <c:f>Knot_Uncached_Data!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Forward Lookup with UDP</c:v>
+                  <c:v>Forware Lookup with UDP</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Forward Lookup with DoT</c:v>
+                  <c:v>Forware Lookup with DoT</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Anonymized Forward Lookup with DoT</c:v>
@@ -259,18 +497,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Uncached!$B$2:$B$4</c:f>
+              <c:f>Knot_Uncached_Data!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.5999999999999999E-2</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2000000000000003E-2</c:v>
+                  <c:v>3.3000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2999999999999997E-2</c:v>
+                  <c:v>3.3000000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -281,7 +519,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Uncached!$C$1</c:f>
+              <c:f>Knot_Uncached_Data!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -302,14 +540,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Uncached!$A$2:$A$4</c:f>
+              <c:f>Knot_Uncached_Data!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Forward Lookup with UDP</c:v>
+                  <c:v>Forware Lookup with UDP</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Forward Lookup with DoT</c:v>
+                  <c:v>Forware Lookup with DoT</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Anonymized Forward Lookup with DoT</c:v>
@@ -319,18 +557,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Uncached!$C$2:$C$4</c:f>
+              <c:f>Knot_Uncached_Data!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.106</c:v>
+                  <c:v>9.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.115</c:v>
+                  <c:v>0.123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.126</c:v>
+                  <c:v>0.128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,11 +584,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="558897496"/>
-        <c:axId val="558909256"/>
+        <c:axId val="526472528"/>
+        <c:axId val="526469784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="558897496"/>
+        <c:axId val="526472528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,7 +631,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="558909256"/>
+        <c:crossAx val="526469784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -401,7 +639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="558909256"/>
+        <c:axId val="526469784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +690,340 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="558897496"/>
+        <c:crossAx val="526472528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Unbound_Uncached_Data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Unbound_Uncached_Data!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Forward Lookup with UDP</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Forward Lookup with DoT</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Anonymized Forward Lookup with DoT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Unbound_Uncached_Data!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2999999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Unbound_Uncached_Data!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Unbound_Uncached_Data!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Forward Lookup with UDP</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Forward Lookup with DoT</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Anonymized Forward Lookup with DoT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Unbound_Uncached_Data!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.115</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.126</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="519149520"/>
+        <c:axId val="519149912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="519149520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="519149912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="519149912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="519149520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -523,7 +1094,528 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Forward Lookup with UDP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet3!$C$10:$F$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Min</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Avg</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Min</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Avg</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unbound</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Knot Resolver</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.106</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Forward Lookup with DoT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet3!$C$10:$F$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Min</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Avg</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Min</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Avg</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unbound</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Knot Resolver</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.115</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anonymized Forward Lookup with DoT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet3!$C$10:$F$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Min</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Avg</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Min</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Avg</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Unbound</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Knot Resolver</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$14:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.2999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.126</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="117393160"/>
+        <c:axId val="117395120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="117393160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="117395120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="117395120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="117393160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1066,11 +2158,1028 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1078,11 +3187,76 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9308523" cy="6090227"/>
+    <xdr:ext cx="9302518" cy="6076533"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9302518" cy="6076533"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9302518" cy="6076533"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1106,20 +3280,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H9" totalsRowShown="0">
-  <autoFilter ref="A1:H9"/>
-  <sortState ref="A2:H9">
-    <sortCondition ref="C1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15"/>
+  <sortState ref="A2:I15">
+    <sortCondition ref="D1:D15"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Resolver IP"/>
-    <tableColumn id="2" name="Resolver Type"/>
+  <tableColumns count="9">
+    <tableColumn id="9" name="Software"/>
+    <tableColumn id="1" name="IP"/>
+    <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Request Type"/>
     <tableColumn id="4" name="Min"/>
     <tableColumn id="5" name="Avg"/>
     <tableColumn id="6" name="Max"/>
     <tableColumn id="7" name="Std.Dev"/>
     <tableColumn id="8" name="Reliab%"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F4" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:F4"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Type"/>
+    <tableColumn id="2" name="Min" dataDxfId="3"/>
+    <tableColumn id="3" name="Avg" dataDxfId="2"/>
+    <tableColumn id="4" name="Max" dataDxfId="1"/>
+    <tableColumn id="5" name="Std.Dev" dataDxfId="0"/>
+    <tableColumn id="6" name="Reliab%"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F4" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:F4"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Resolver Type"/>
+    <tableColumn id="2" name="Min"/>
+    <tableColumn id="3" name="Avg"/>
+    <tableColumn id="4" name="Max"/>
+    <tableColumn id="5" name="Std.Dev"/>
+    <tableColumn id="6" name="Reliab%"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1388,252 +3593,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H2">
+        <v>2E-3</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>0.02</v>
+      </c>
+      <c r="F3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="H3">
+        <v>1E-3</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="E2">
-        <v>1.2E-2</v>
-      </c>
-      <c r="F2">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="G2">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F4">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="H4">
         <v>2E-3</v>
       </c>
-      <c r="H2">
+      <c r="I4">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
         <v>0.02</v>
       </c>
-      <c r="E3">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="F3">
-        <v>2.7E-2</v>
-      </c>
-      <c r="G3">
-        <v>1E-3</v>
-      </c>
-      <c r="H3">
+      <c r="F5">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H5">
+        <v>2E-3</v>
+      </c>
+      <c r="I5">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>1.9E-2</v>
-      </c>
-      <c r="E4">
-        <v>2.3E-2</v>
-      </c>
-      <c r="F4">
-        <v>3.1E-2</v>
-      </c>
-      <c r="G4">
-        <v>2E-3</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>0.02</v>
-      </c>
-      <c r="E5">
-        <v>2.3E-2</v>
-      </c>
-      <c r="F5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="G5">
-        <v>2E-3</v>
-      </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>0.02</v>
+      </c>
+      <c r="F6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G6">
+        <v>2.7E-2</v>
+      </c>
+      <c r="H6">
+        <v>1E-3</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>0.02</v>
+      </c>
+      <c r="F7">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G7">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>1E-3</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>0.02</v>
+      </c>
+      <c r="F8">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G8">
+        <v>2.7E-2</v>
+      </c>
+      <c r="H8">
+        <v>1E-3</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="E6">
+      <c r="F9">
         <v>0.188</v>
       </c>
-      <c r="F6">
+      <c r="G9">
         <v>0.35</v>
       </c>
-      <c r="G6">
+      <c r="H9">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="H6">
+      <c r="I9">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.106</v>
+      </c>
+      <c r="G10">
+        <v>0.432</v>
+      </c>
+      <c r="H10">
+        <v>0.109</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="E7">
-        <v>0.106</v>
-      </c>
-      <c r="F7">
-        <v>0.432</v>
-      </c>
-      <c r="G7">
-        <v>0.109</v>
-      </c>
-      <c r="H7">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.115</v>
+      </c>
+      <c r="G11">
+        <v>0.375</v>
+      </c>
+      <c r="H11">
+        <v>0.09</v>
+      </c>
+      <c r="I11">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="E8">
-        <v>0.115</v>
-      </c>
-      <c r="F8">
-        <v>0.375</v>
-      </c>
-      <c r="G8">
-        <v>0.09</v>
-      </c>
-      <c r="H8">
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.126</v>
+      </c>
+      <c r="G12">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="H12">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I12">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="E9">
-        <v>0.126</v>
-      </c>
-      <c r="F9">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="G9">
-        <v>9.4E-2</v>
-      </c>
-      <c r="H9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F13">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G13">
+        <v>0.313</v>
+      </c>
+      <c r="H13">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.123</v>
+      </c>
+      <c r="G14">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="H14">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.128</v>
+      </c>
+      <c r="G15">
+        <v>0.628</v>
+      </c>
+      <c r="H15">
+        <v>0.125</v>
+      </c>
+      <c r="I15">
         <v>100</v>
       </c>
     </row>
@@ -1650,7 +4057,113 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F4" sqref="A2:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.313</v>
+      </c>
+      <c r="E2" s="4">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.123</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.128</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.628</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="F4" s="8">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,90 +4171,384 @@
     <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" customWidth="1"/>
-    <col min="4" max="5" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="4">
         <v>0.106</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="4">
         <v>0.432</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="4">
         <v>0.109</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="5">
         <v>0.115</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="5">
         <v>0.375</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>0.09</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="9">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="9">
         <v>0.126</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="9">
         <v>0.36899999999999999</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="9">
         <v>9.4E-2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="8">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="14">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.106</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0.432</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0.109</v>
+      </c>
+      <c r="G2" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="14">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.115</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="G3" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="14">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.126</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="F4" s="14">
+        <v>9.4E-2</v>
+      </c>
+      <c r="G4" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D5" s="9">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.313</v>
+      </c>
+      <c r="F5" s="9">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G5" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="14">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.123</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G6" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.128</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.628</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="G7" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0.106</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0.115</v>
+      </c>
+      <c r="E13" s="14">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0.123</v>
+      </c>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="14">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0.126</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.128</v>
+      </c>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="G17" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>